<commit_message>
close #161: Add check for indicators described in proportionalities
</commit_message>
<xml_diff>
--- a/input_data/data_ground_truth_01/proporcionalidades.xlsx
+++ b/input_data/data_ground_truth_01/proporcionalidades.xlsx
@@ -20,51 +20,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
-  <si>
-    <t xml:space="preserve">5008-2010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5009-2010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5010-2010</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="18">
+  <si>
+    <t xml:space="preserve">2-2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-2030-O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-2050-O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-2030-P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-2050-P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5-2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5-2030-O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5-2050-O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5-2030-P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5-2050-P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6-2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7-2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8-2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9-2015</t>
   </si>
   <si>
     <t xml:space="preserve">id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5021-2010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5022-2010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5023-2010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5024-2010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5025-2010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5026-2010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5027-2010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5028-2010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5029-2010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5030-2010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5031-2010</t>
   </si>
   <si>
     <t xml:space="preserve">DI</t>
@@ -77,7 +83,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -105,6 +111,13 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -149,17 +162,25 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -285,74 +306,294 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:BH6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P2" activeCellId="0" sqref="P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.34375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="2" style="1" width="9.92"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="1" style="1" width="16.34"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="48" min="13" style="2" width="16.34"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="60" min="49" style="1" width="16.34"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="61" style="2" width="16.34"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2" t="s">
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="3"/>
+      <c r="AC1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD1" s="3"/>
+      <c r="AE1" s="3"/>
+      <c r="AF1" s="3"/>
+      <c r="AG1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH1" s="3"/>
+      <c r="AI1" s="3"/>
+      <c r="AJ1" s="3"/>
+      <c r="AK1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AL1" s="3"/>
+      <c r="AM1" s="3"/>
+      <c r="AN1" s="3"/>
+      <c r="AO1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AP1" s="3"/>
+      <c r="AQ1" s="3"/>
+      <c r="AR1" s="3"/>
+      <c r="AS1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AT1" s="3"/>
+      <c r="AU1" s="3"/>
+      <c r="AV1" s="3"/>
+      <c r="AW1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AX1" s="3"/>
+      <c r="AY1" s="3"/>
+      <c r="AZ1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="BA1" s="3"/>
+      <c r="BB1" s="3"/>
+      <c r="BC1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="BD1" s="3"/>
+      <c r="BE1" s="3"/>
+      <c r="BF1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="BG1" s="3"/>
+      <c r="BH1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="S2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="T2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="U2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AL2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AN2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AO2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AP2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AQ2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AS2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AT2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AU2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AV2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AW2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="AX2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AY2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>14</v>
+      <c r="AZ2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="BA2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="BB2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="BC2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="BD2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="BE2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="BF2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="BG2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="BH2" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -372,7 +613,7 @@
         <v>0.442</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G3" s="1" t="n">
         <v>0.558</v>
@@ -391,6 +632,150 @@
       </c>
       <c r="L3" s="1" t="n">
         <v>0.164</v>
+      </c>
+      <c r="M3" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="N3" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="O3" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="P3" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="Q3" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="R3" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="S3" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="T3" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="U3" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="V3" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="W3" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="X3" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="Y3" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="Z3" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="AA3" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="AB3" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="AC3" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="AD3" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="AE3" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="AF3" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="AG3" s="1" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AI3" s="1" t="n">
+        <v>0.558</v>
+      </c>
+      <c r="AJ3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="AL3" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="AM3" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="AN3" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="AO3" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="AP3" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="AQ3" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="AR3" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="AS3" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="AT3" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="AU3" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="AV3" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="AW3" s="1" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="AX3" s="1" t="n">
+        <v>0.347</v>
+      </c>
+      <c r="AY3" s="1" t="n">
+        <v>0.211</v>
+      </c>
+      <c r="AZ3" s="1" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="BA3" s="1" t="n">
+        <v>0.347</v>
+      </c>
+      <c r="BB3" s="1" t="n">
+        <v>0.211</v>
+      </c>
+      <c r="BC3" s="1" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="BD3" s="1" t="n">
+        <v>0.347</v>
+      </c>
+      <c r="BE3" s="1" t="n">
+        <v>0.211</v>
+      </c>
+      <c r="BF3" s="1" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="BG3" s="1" t="n">
+        <v>0.347</v>
+      </c>
+      <c r="BH3" s="1" t="n">
+        <v>0.211</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -410,7 +795,7 @@
         <v>0.442</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G4" s="1" t="n">
         <v>0.558</v>
@@ -429,6 +814,150 @@
       </c>
       <c r="L4" s="1" t="n">
         <v>0.164</v>
+      </c>
+      <c r="M4" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="N4" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="O4" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="P4" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="Q4" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="R4" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="S4" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="T4" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="U4" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="V4" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="W4" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="X4" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="Y4" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="Z4" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="AA4" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="AB4" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="AC4" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="AD4" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="AE4" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="AF4" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="AG4" s="1" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AI4" s="1" t="n">
+        <v>0.558</v>
+      </c>
+      <c r="AJ4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="AL4" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="AM4" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="AN4" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="AO4" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="AP4" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="AQ4" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="AR4" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="AS4" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="AT4" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="AU4" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="AV4" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="AW4" s="1" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="AX4" s="1" t="n">
+        <v>0.347</v>
+      </c>
+      <c r="AY4" s="1" t="n">
+        <v>0.211</v>
+      </c>
+      <c r="AZ4" s="1" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="BA4" s="1" t="n">
+        <v>0.347</v>
+      </c>
+      <c r="BB4" s="1" t="n">
+        <v>0.211</v>
+      </c>
+      <c r="BC4" s="1" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="BD4" s="1" t="n">
+        <v>0.347</v>
+      </c>
+      <c r="BE4" s="1" t="n">
+        <v>0.211</v>
+      </c>
+      <c r="BF4" s="1" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="BG4" s="1" t="n">
+        <v>0.347</v>
+      </c>
+      <c r="BH4" s="1" t="n">
+        <v>0.211</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -448,7 +977,7 @@
         <v>0.442</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>0.558</v>
@@ -467,6 +996,150 @@
       </c>
       <c r="L5" s="1" t="n">
         <v>0.164</v>
+      </c>
+      <c r="M5" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="N5" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="O5" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="P5" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="Q5" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="R5" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="S5" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="T5" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="U5" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="V5" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="W5" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="X5" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="Y5" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="Z5" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="AA5" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="AB5" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="AC5" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="AD5" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="AE5" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="AF5" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="AG5" s="1" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="AH5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AI5" s="1" t="n">
+        <v>0.558</v>
+      </c>
+      <c r="AJ5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK5" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="AL5" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="AM5" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="AN5" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="AO5" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="AP5" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="AQ5" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="AR5" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="AS5" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="AT5" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="AU5" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="AV5" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="AW5" s="1" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="AX5" s="1" t="n">
+        <v>0.347</v>
+      </c>
+      <c r="AY5" s="1" t="n">
+        <v>0.211</v>
+      </c>
+      <c r="AZ5" s="1" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="BA5" s="1" t="n">
+        <v>0.347</v>
+      </c>
+      <c r="BB5" s="1" t="n">
+        <v>0.211</v>
+      </c>
+      <c r="BC5" s="1" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="BD5" s="1" t="n">
+        <v>0.347</v>
+      </c>
+      <c r="BE5" s="1" t="n">
+        <v>0.211</v>
+      </c>
+      <c r="BF5" s="1" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="BG5" s="1" t="n">
+        <v>0.347</v>
+      </c>
+      <c r="BH5" s="1" t="n">
+        <v>0.211</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -486,7 +1159,7 @@
         <v>0.442</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G6" s="1" t="n">
         <v>0.558</v>
@@ -505,6 +1178,150 @@
       </c>
       <c r="L6" s="1" t="n">
         <v>0.164</v>
+      </c>
+      <c r="M6" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="N6" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="O6" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="P6" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="Q6" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="R6" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="S6" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="T6" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="U6" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="V6" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="W6" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="X6" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="Y6" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="Z6" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="AA6" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="AB6" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="AC6" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="AD6" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="AE6" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="AF6" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="AG6" s="1" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="AH6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AI6" s="1" t="n">
+        <v>0.558</v>
+      </c>
+      <c r="AJ6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK6" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="AL6" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="AM6" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="AN6" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="AO6" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="AP6" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="AQ6" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="AR6" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="AS6" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="AT6" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="AU6" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="AV6" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="AW6" s="1" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="AX6" s="1" t="n">
+        <v>0.347</v>
+      </c>
+      <c r="AY6" s="1" t="n">
+        <v>0.211</v>
+      </c>
+      <c r="AZ6" s="1" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="BA6" s="1" t="n">
+        <v>0.347</v>
+      </c>
+      <c r="BB6" s="1" t="n">
+        <v>0.211</v>
+      </c>
+      <c r="BC6" s="1" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="BD6" s="1" t="n">
+        <v>0.347</v>
+      </c>
+      <c r="BE6" s="1" t="n">
+        <v>0.211</v>
+      </c>
+      <c r="BF6" s="1" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="BG6" s="1" t="n">
+        <v>0.347</v>
+      </c>
+      <c r="BH6" s="1" t="n">
+        <v>0.211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
close #21: Checking scenario coherence in valores.xlsx e proporcionalidades.xlsx
</commit_message>
<xml_diff>
--- a/input_data/data_ground_truth_01/proporcionalidades.xlsx
+++ b/input_data/data_ground_truth_01/proporcionalidades.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="18">
   <si>
     <t xml:space="preserve">2-2015</t>
   </si>
@@ -46,43 +46,31 @@
     <t xml:space="preserve">id</t>
   </si>
   <si>
-    <t xml:space="preserve">3-2030-O</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4-2050-O</t>
+    <t xml:space="preserve">4-2015</t>
   </si>
   <si>
     <t xml:space="preserve">5-2030-P</t>
   </si>
   <si>
-    <t xml:space="preserve">3-2050-O</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4-2030-P</t>
+    <t xml:space="preserve">5-2050-O</t>
   </si>
   <si>
     <t xml:space="preserve">5-2050-P</t>
   </si>
   <si>
-    <t xml:space="preserve">6-2030-O</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6-2050-O</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7-2030-P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7-2050-P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8-2030-O</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9-2030-O</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9-2050-O</t>
+    <t xml:space="preserve">5-2030-O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5-2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7-2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8-2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9-2015</t>
   </si>
   <si>
     <t xml:space="preserve">DI</t>
@@ -315,16 +303,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AA6"/>
+  <dimension ref="A1:X6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y1" activeCellId="0" sqref="Y1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.34375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16350" min="1" style="1" width="16.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16351" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16347" min="1" style="1" width="16.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16348" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -362,95 +350,83 @@
         <v>5</v>
       </c>
       <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
+      <c r="W1" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="X1" s="2"/>
-      <c r="Y1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="Z1" s="2"/>
-      <c r="AA1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="I2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="T2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="U2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="V2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -470,7 +446,7 @@
         <v>0.442</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G3" s="1" t="n">
         <v>0.558</v>
@@ -515,25 +491,16 @@
         <v>0.164</v>
       </c>
       <c r="U3" s="1" t="n">
-        <v>0.506</v>
+        <v>0.738</v>
       </c>
       <c r="V3" s="1" t="n">
-        <v>0.232</v>
+        <v>0.262</v>
       </c>
       <c r="W3" s="1" t="n">
-        <v>0.098</v>
+        <v>0.442</v>
       </c>
       <c r="X3" s="1" t="n">
-        <v>0.164</v>
-      </c>
-      <c r="Y3" s="1" t="n">
-        <v>0.442</v>
-      </c>
-      <c r="Z3" s="1" t="n">
-        <v>0.347</v>
-      </c>
-      <c r="AA3" s="1" t="n">
-        <v>0.211</v>
+        <v>0.558</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -553,7 +520,7 @@
         <v>0.442</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G4" s="1" t="n">
         <v>0.558</v>
@@ -598,25 +565,16 @@
         <v>0.164</v>
       </c>
       <c r="U4" s="1" t="n">
-        <v>0.506</v>
+        <v>0.738</v>
       </c>
       <c r="V4" s="1" t="n">
-        <v>0.232</v>
+        <v>0.262</v>
       </c>
       <c r="W4" s="1" t="n">
-        <v>0.098</v>
+        <v>0.442</v>
       </c>
       <c r="X4" s="1" t="n">
-        <v>0.164</v>
-      </c>
-      <c r="Y4" s="1" t="n">
-        <v>0.442</v>
-      </c>
-      <c r="Z4" s="1" t="n">
-        <v>0.347</v>
-      </c>
-      <c r="AA4" s="1" t="n">
-        <v>0.211</v>
+        <v>0.558</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -636,7 +594,7 @@
         <v>0.442</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>0.558</v>
@@ -681,25 +639,16 @@
         <v>0.164</v>
       </c>
       <c r="U5" s="1" t="n">
-        <v>0.506</v>
+        <v>0.738</v>
       </c>
       <c r="V5" s="1" t="n">
-        <v>0.232</v>
+        <v>0.262</v>
       </c>
       <c r="W5" s="1" t="n">
-        <v>0.098</v>
+        <v>0.442</v>
       </c>
       <c r="X5" s="1" t="n">
-        <v>0.164</v>
-      </c>
-      <c r="Y5" s="1" t="n">
-        <v>0.442</v>
-      </c>
-      <c r="Z5" s="1" t="n">
-        <v>0.347</v>
-      </c>
-      <c r="AA5" s="1" t="n">
-        <v>0.211</v>
+        <v>0.558</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -719,7 +668,7 @@
         <v>0.442</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G6" s="1" t="n">
         <v>0.558</v>
@@ -764,25 +713,16 @@
         <v>0.164</v>
       </c>
       <c r="U6" s="1" t="n">
-        <v>0.506</v>
+        <v>0.738</v>
       </c>
       <c r="V6" s="1" t="n">
-        <v>0.232</v>
+        <v>0.262</v>
       </c>
       <c r="W6" s="1" t="n">
-        <v>0.098</v>
+        <v>0.442</v>
       </c>
       <c r="X6" s="1" t="n">
-        <v>0.164</v>
-      </c>
-      <c r="Y6" s="1" t="n">
-        <v>0.442</v>
-      </c>
-      <c r="Z6" s="1" t="n">
-        <v>0.347</v>
-      </c>
-      <c r="AA6" s="1" t="n">
-        <v>0.211</v>
+        <v>0.558</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
close #150: Improves the logic of checking mandatory and unnecessary columns for 'values.xlsx' and 'proportionalities.xlsx'
</commit_message>
<xml_diff>
--- a/input_data/data_ground_truth_01/proporcionalidades.xlsx
+++ b/input_data/data_ground_truth_01/proporcionalidades.xlsx
@@ -305,8 +305,8 @@
   </sheetPr>
   <dimension ref="A1:X6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U13" activeCellId="0" sqref="U13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.34375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>